<commit_message>
Revert "update Todo/Bug form"
This reverts commit ed2183e278a6ca23c45f87f02d31c3b70ccf840c.
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
-  <workbookPr filterPrivacy="1" showInkAnnotation="0"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Todo List" sheetId="1" r:id="rId1"/>
-    <sheet name="Bug List" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ToDo List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -223,10 +222,6 @@
       </rPr>
       <t>时，最好可以自动把左侧的相应寄存器也选中</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>open</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -234,7 +229,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,51 +269,16 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -326,66 +286,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -421,13 +329,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -470,13 +372,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -768,8 +664,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:B10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -777,17 +672,16 @@
     <col min="1" max="1" width="63.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:2" ht="15">
-      <c r="A2" s="4" t="s">
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -795,64 +689,40 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -876,26 +746,11 @@
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Feature updated for No2.4.6.7
Detail in ToDo list documentations.
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>ToDo List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -222,13 +222,33 @@
       </rPr>
       <t>时，最好可以自动把左侧的相应寄存器也选中</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comments</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>左侧预留出空间，并在显示的时候左侧也预留两个空格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整行加了个灰色背景</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -291,13 +311,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -335,7 +361,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -378,7 +404,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -441,7 +467,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -476,7 +502,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -653,77 +679,354 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="63.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="3:3">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="3:3">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="3:3">
+      <c r="C19" s="3"/>
+    </row>
+    <row r="20" spans="3:3">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="3:3">
+      <c r="C21" s="3"/>
+    </row>
+    <row r="22" spans="3:3">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="3:3">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="3:3">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="3:3">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="3:3">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="3:3">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="3:3">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="3:3">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="3:3">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="3:3">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" s="3"/>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="3:3">
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="3:3">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="3:3">
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="3:3">
+      <c r="C63" s="3"/>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64" s="3"/>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="3:3">
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="3:3">
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="3:3">
+      <c r="C71" s="3"/>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72" s="3"/>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="3:3">
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="3:3">
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="3:3">
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="3:3">
+      <c r="C79" s="3"/>
+    </row>
+    <row r="80" spans="3:3">
+      <c r="C80" s="3"/>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82" s="3"/>
+    </row>
+    <row r="83" spans="3:3">
+      <c r="C83" s="3"/>
+    </row>
+    <row r="84" spans="3:3">
+      <c r="C84" s="3"/>
+    </row>
+    <row r="85" spans="3:3">
+      <c r="C85" s="3"/>
+    </row>
+    <row r="86" spans="3:3">
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87" spans="3:3">
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88" spans="3:3">
+      <c r="C88" s="3"/>
+    </row>
+    <row r="89" spans="3:3">
+      <c r="C89" s="3"/>
+    </row>
+    <row r="90" spans="3:3">
+      <c r="C90" s="3"/>
+    </row>
+    <row r="91" spans="3:3">
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92" spans="3:3">
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -737,12 +1040,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -751,15 +1056,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Item No5. 10, 11 and 12
Added Customer tab edit(Add or Remove);
Made search window also set background for RegName
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240"/>
@@ -13,8 +13,8 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>ToDo List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -416,13 +416,21 @@
   </si>
   <si>
     <t>Normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鼠标按住圈选就可以了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -564,10 +572,24 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -615,7 +637,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -664,7 +686,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -713,7 +735,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -722,10 +744,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -745,7 +767,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1014,22 +1036,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="63.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.5" style="1" bestFit="1" customWidth="1"/>
@@ -1043,7 +1065,7 @@
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1">
+    <row r="2" spans="1:4" ht="14.25" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
@@ -1057,7 +1079,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickTop="1">
+    <row r="3" spans="1:4" ht="14.25" thickTop="1">
       <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
@@ -1104,7 +1126,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>23</v>
@@ -1155,14 +1177,16 @@
       <c r="C11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>24</v>
@@ -1174,7 +1198,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>24</v>
@@ -1186,7 +1210,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>24</v>
@@ -1538,12 +1562,12 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B3:C40">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="open">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="open">
       <formula>NOT(ISERROR(SEARCH("open",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:C42">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="done">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="done">
       <formula>NOT(ISERROR(SEARCH("done",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1558,14 +1582,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1574,12 +1596,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A6" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1589,15 +1611,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added bfValue and regValue changing binding
Also added bfvalue and reg value input formate validation check which is
very important to make the GUI looks fancy.
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>ToDo List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -424,6 +424,30 @@
   </si>
   <si>
     <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>No.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Add selected write(right click menu)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Update GUI display when selected read</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Save project</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Import &amp; Export reg setting</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -575,21 +599,7 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -637,7 +647,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -686,7 +696,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -735,7 +745,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -747,7 +757,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -767,7 +777,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1036,7 +1046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1044,537 +1054,610 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="63.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="4"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
       <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" ht="14.25" thickBot="1">
-      <c r="A2" s="5" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.25" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.25" thickTop="1">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:5" ht="14.25" thickTop="1">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="7" t="s">
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="7" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="7" t="s">
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="7" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="9" t="s">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="7" t="s">
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="9" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>17</v>
-      </c>
       <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="E11" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="7" t="s">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="D13" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="7" t="s">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="D14" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="7"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
       <c r="B15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
       <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="8"/>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="7"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
       <c r="B17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="7"/>
+        <v>31</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
       <c r="B18" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="D40" s="2"/>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="D42" s="2"/>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="D45" s="2"/>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="D46" s="2"/>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="D47" s="2"/>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="D48" s="2"/>
-    </row>
-    <row r="49" spans="4:4">
-      <c r="D49" s="2"/>
-    </row>
-    <row r="50" spans="4:4">
-      <c r="D50" s="2"/>
-    </row>
-    <row r="51" spans="4:4">
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="4:4">
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="4:4">
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="4:4">
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="4:4">
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="4:4">
-      <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="4:4">
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="4:4">
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="4:4">
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="4:4">
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="4:4">
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="4:4">
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="4:4">
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="4:4">
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="4:4">
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="4:4">
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="4:4">
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="4:4">
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="4:4">
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="4:4">
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="4:4">
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="4:4">
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="4:4">
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="4:4">
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="4:4">
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="4:4">
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="4:4">
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="4:4">
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="4:4">
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="4:4">
-      <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="4:4">
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="4:4">
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="4:4">
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="4:4">
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="4:4">
-      <c r="D85" s="2"/>
-    </row>
-    <row r="86" spans="4:4">
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="4:4">
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="4:4">
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="4:4">
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="4:4">
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="4:4">
-      <c r="D91" s="2"/>
-    </row>
-    <row r="92" spans="4:4">
-      <c r="D92" s="2"/>
-    </row>
-    <row r="93" spans="4:4">
-      <c r="D93" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="B30" s="7"/>
+      <c r="C30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="2:5">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="2:5">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="2:5">
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="E40" s="2"/>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="2:5">
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="2:5">
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="2:5">
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" spans="2:5">
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" spans="2:5">
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" spans="2:5">
+      <c r="E48" s="2"/>
+    </row>
+    <row r="49" spans="5:5">
+      <c r="E49" s="2"/>
+    </row>
+    <row r="50" spans="5:5">
+      <c r="E50" s="2"/>
+    </row>
+    <row r="51" spans="5:5">
+      <c r="E51" s="2"/>
+    </row>
+    <row r="52" spans="5:5">
+      <c r="E52" s="2"/>
+    </row>
+    <row r="53" spans="5:5">
+      <c r="E53" s="2"/>
+    </row>
+    <row r="54" spans="5:5">
+      <c r="E54" s="2"/>
+    </row>
+    <row r="55" spans="5:5">
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="5:5">
+      <c r="E56" s="2"/>
+    </row>
+    <row r="57" spans="5:5">
+      <c r="E57" s="2"/>
+    </row>
+    <row r="58" spans="5:5">
+      <c r="E58" s="2"/>
+    </row>
+    <row r="59" spans="5:5">
+      <c r="E59" s="2"/>
+    </row>
+    <row r="60" spans="5:5">
+      <c r="E60" s="2"/>
+    </row>
+    <row r="61" spans="5:5">
+      <c r="E61" s="2"/>
+    </row>
+    <row r="62" spans="5:5">
+      <c r="E62" s="2"/>
+    </row>
+    <row r="63" spans="5:5">
+      <c r="E63" s="2"/>
+    </row>
+    <row r="64" spans="5:5">
+      <c r="E64" s="2"/>
+    </row>
+    <row r="65" spans="5:5">
+      <c r="E65" s="2"/>
+    </row>
+    <row r="66" spans="5:5">
+      <c r="E66" s="2"/>
+    </row>
+    <row r="67" spans="5:5">
+      <c r="E67" s="2"/>
+    </row>
+    <row r="68" spans="5:5">
+      <c r="E68" s="2"/>
+    </row>
+    <row r="69" spans="5:5">
+      <c r="E69" s="2"/>
+    </row>
+    <row r="70" spans="5:5">
+      <c r="E70" s="2"/>
+    </row>
+    <row r="71" spans="5:5">
+      <c r="E71" s="2"/>
+    </row>
+    <row r="72" spans="5:5">
+      <c r="E72" s="2"/>
+    </row>
+    <row r="73" spans="5:5">
+      <c r="E73" s="2"/>
+    </row>
+    <row r="74" spans="5:5">
+      <c r="E74" s="2"/>
+    </row>
+    <row r="75" spans="5:5">
+      <c r="E75" s="2"/>
+    </row>
+    <row r="76" spans="5:5">
+      <c r="E76" s="2"/>
+    </row>
+    <row r="77" spans="5:5">
+      <c r="E77" s="2"/>
+    </row>
+    <row r="78" spans="5:5">
+      <c r="E78" s="2"/>
+    </row>
+    <row r="79" spans="5:5">
+      <c r="E79" s="2"/>
+    </row>
+    <row r="80" spans="5:5">
+      <c r="E80" s="2"/>
+    </row>
+    <row r="81" spans="5:5">
+      <c r="E81" s="2"/>
+    </row>
+    <row r="82" spans="5:5">
+      <c r="E82" s="2"/>
+    </row>
+    <row r="83" spans="5:5">
+      <c r="E83" s="2"/>
+    </row>
+    <row r="84" spans="5:5">
+      <c r="E84" s="2"/>
+    </row>
+    <row r="85" spans="5:5">
+      <c r="E85" s="2"/>
+    </row>
+    <row r="86" spans="5:5">
+      <c r="E86" s="2"/>
+    </row>
+    <row r="87" spans="5:5">
+      <c r="E87" s="2"/>
+    </row>
+    <row r="88" spans="5:5">
+      <c r="E88" s="2"/>
+    </row>
+    <row r="89" spans="5:5">
+      <c r="E89" s="2"/>
+    </row>
+    <row r="90" spans="5:5">
+      <c r="E90" s="2"/>
+    </row>
+    <row r="91" spans="5:5">
+      <c r="E91" s="2"/>
+    </row>
+    <row r="92" spans="5:5">
+      <c r="E92" s="2"/>
+    </row>
+    <row r="93" spans="5:5">
+      <c r="E93" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B3:C40">
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="open">
-      <formula>NOT(ISERROR(SEARCH("open",B3)))</formula>
+  <conditionalFormatting sqref="C3:D40">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="open">
+      <formula>NOT(ISERROR(SEARCH("open",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:C42">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="done">
-      <formula>NOT(ISERROR(SEARCH("done",B3)))</formula>
+  <conditionalFormatting sqref="C3:D42">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="done">
+      <formula>NOT(ISERROR(SEARCH("done",C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A8" location="Sheet2!A1" display="6. 红框位置留出一些空间"/>
-    <hyperlink ref="A9" location="Sheet3!A1" display="7. 显示寄存器名称，在图示位置，可以考虑加粗字体，左对齐来区别"/>
-    <hyperlink ref="A11" location="Sheet4!A1" display="9. 'selected read', 如何选中，是否可以加上checkBox"/>
+    <hyperlink ref="B8" location="Sheet2!A1" display="6. 红框位置留出一些空间"/>
+    <hyperlink ref="B9" location="Sheet3!A1" display="7. 显示寄存器名称，在图示位置，可以考虑加粗字体，左对齐来区别"/>
+    <hyperlink ref="B11" location="Sheet4!A1" display="9. 'selected read', 如何选中，是否可以加上checkBox"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Import and Export functions.And fixed a bug
The bug is that when using the bfvalue with 0x, GUI will crash.
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>ToDo List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -448,6 +448,22 @@
   </si>
   <si>
     <t>Import &amp; Export reg setting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync Noramal tabs and Customer tab </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When register modified in customer, then should update other tab which contains the same register.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Difficult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -569,7 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -593,6 +609,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -647,7 +669,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -696,7 +718,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -745,7 +767,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -757,7 +779,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -777,7 +799,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1046,7 +1068,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1058,14 +1080,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="52.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1276,7 +1299,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
@@ -1289,7 +1312,7 @@
         <v>29</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
@@ -1320,16 +1343,22 @@
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="27">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+      <c r="B19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1">

</xml_diff>

<commit_message>
Revert "Added Import and Export functions.And fixed a bug"
This reverts commit bf6ac1c9a83549d5aac476b0a5395d488dae48da.
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>ToDo List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -448,22 +448,6 @@
   </si>
   <si>
     <t>Import &amp; Export reg setting</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Sync Noramal tabs and Customer tab </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>When register modified in customer, then should update other tab which contains the same register.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Difficult</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -585,7 +569,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -609,12 +593,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -669,7 +647,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -718,7 +696,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -767,7 +745,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -779,7 +757,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -799,7 +777,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1068,7 +1046,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1080,15 +1058,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" customWidth="1"/>
-    <col min="5" max="5" width="52.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1299,7 +1276,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
@@ -1312,7 +1289,7 @@
         <v>29</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
@@ -1343,22 +1320,16 @@
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="27">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>34</v>
-      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1">

</xml_diff>

<commit_message>
Revert "Revert "Added Import and Export functions.And fixed a bug""
This reverts commit 715ba4c78a77b642d772f027522e49f33da0c56b.

# Conflicts:

#	MDEvaPlatform/MDEva/obj/x86/Debug/DesignTimeResolveAssemblyReferences.cache
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>ToDo List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -448,6 +448,22 @@
   </si>
   <si>
     <t>Import &amp; Export reg setting</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Sync Noramal tabs and Customer tab </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When register modified in customer, then should update other tab which contains the same register.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Difficult</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -569,7 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -593,6 +609,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -647,7 +669,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -696,7 +718,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -745,7 +767,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -757,7 +779,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -777,7 +799,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1046,7 +1068,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1058,14 +1080,15 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" customWidth="1"/>
+    <col min="5" max="5" width="52.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1276,7 +1299,7 @@
         <v>30</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8"/>
@@ -1289,7 +1312,7 @@
         <v>29</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
@@ -1320,16 +1343,22 @@
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" ht="27">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+      <c r="B19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="1">

</xml_diff>

<commit_message>
update todo list after review with RPan
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240"/>
@@ -13,8 +13,8 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t>ToDo List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -464,13 +464,89 @@
   </si>
   <si>
     <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置可以多个customer Tab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>tab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>之间的数据</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sync</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>记录操作</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高亮bitfield的描述，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>command operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最基本的读写操作，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>支持多byte操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>折叠</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示项目名称，在状态栏或者标题处</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -585,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -616,10 +692,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -669,7 +746,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -718,7 +795,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -767,7 +844,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -779,7 +856,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -799,7 +876,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1068,22 +1145,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.125" bestFit="1" customWidth="1"/>
@@ -1100,7 +1177,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" thickBot="1">
+    <row r="2" spans="1:5" ht="15" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1117,7 +1194,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" thickTop="1">
+    <row r="3" spans="1:5" ht="15" thickTop="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1343,7 +1420,7 @@
       <c r="D18" s="7"/>
       <c r="E18" s="8"/>
     </row>
-    <row r="19" spans="1:5" ht="27">
+    <row r="19" spans="1:5" ht="28.5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1364,7 +1441,9 @@
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="7"/>
+      <c r="B20" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="C20" s="7" t="s">
         <v>17</v>
       </c>
@@ -1375,7 +1454,9 @@
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="7"/>
+      <c r="B21" s="7" t="s">
+        <v>38</v>
+      </c>
       <c r="C21" s="7" t="s">
         <v>17</v>
       </c>
@@ -1386,7 +1467,9 @@
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="7"/>
+      <c r="B22" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="C22" s="7" t="s">
         <v>17</v>
       </c>
@@ -1394,7 +1477,9 @@
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5">
-      <c r="B23" s="7"/>
+      <c r="B23" s="14" t="s">
+        <v>40</v>
+      </c>
       <c r="C23" s="7" t="s">
         <v>17</v>
       </c>
@@ -1402,23 +1487,33 @@
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5">
-      <c r="B24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="C24" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5">
-      <c r="B25" s="7"/>
+      <c r="B25" s="14" t="s">
+        <v>42</v>
+      </c>
       <c r="C25" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5">
-      <c r="B26" s="7"/>
+      <c r="B26" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="C26" s="7" t="s">
         <v>17</v>
       </c>
@@ -1426,7 +1521,9 @@
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5">
-      <c r="B27" s="7"/>
+      <c r="B27" s="14" t="s">
+        <v>45</v>
+      </c>
       <c r="C27" s="7" t="s">
         <v>17</v>
       </c>
@@ -1434,11 +1531,15 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="B28" s="7"/>
+      <c r="B28" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="C28" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5">
@@ -1694,12 +1795,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1708,12 +1809,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1723,12 +1824,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Regmap dand GUI display after importing.
Also and condition in import and export func. If no project open, this
functions is disabled.
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -543,11 +543,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>partly Done</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Can export, but doesn't update GUI and regmap after import</t>
+    <t>Done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Waiting test with Hardware</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -762,7 +762,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -811,7 +811,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -860,7 +860,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -872,7 +872,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -892,7 +892,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1161,7 +1161,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1173,7 +1173,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1431,11 +1431,11 @@
         <v>32</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="27">
@@ -1521,13 +1521,13 @@
         <v>42</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>44</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5">

</xml_diff>

<commit_message>
Init dongle, add connect button
</commit_message>
<xml_diff>
--- a/MDEvaPlatform/ToDo.xlsx
+++ b/MDEvaPlatform/ToDo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="12240"/>
@@ -13,8 +13,8 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
   <si>
     <t>ToDo List</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -543,26 +543,169 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Done</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Waiting test with Hardware</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Waiting test with Hardware</t>
+    <r>
+      <t xml:space="preserve">testTab, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>需要先写</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>，才能操作相应寄存器</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这个key如何在regmap中定义？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>bitfield</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>跨</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>byte</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>时，描述会两个地方都是整体描述</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>这么操作是否OK？</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Regmap </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>导入的时候改成用</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Reg Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>来识别</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（目前方案是搜索包含  Reg字符串</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可以通过表头来筛选是否显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>Tab</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>中的列是否显示需要筛选</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改寄存器值，同意由“写”命令执行写操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5">
     <font>
       <sz val="11"/>
@@ -604,7 +747,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,6 +757,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -677,7 +826,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -709,10 +858,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -762,7 +915,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -811,7 +964,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -860,7 +1013,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D49AF51-F530-4C1F-8580-3F8E506B51D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -872,7 +1025,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -892,7 +1045,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1161,22 +1314,22 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="2" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="63.125" bestFit="1" customWidth="1"/>
@@ -1193,7 +1346,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" ht="14.25" thickBot="1">
+    <row r="2" spans="1:5" ht="15" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1210,7 +1363,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.25" thickTop="1">
+    <row r="3" spans="1:5" ht="15" thickTop="1">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1431,14 +1584,12 @@
         <v>32</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="27">
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" ht="28.5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1495,6 +1646,9 @@
       <c r="E22" s="8"/>
     </row>
     <row r="23" spans="1:5">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
       <c r="B23" s="14" t="s">
         <v>40</v>
       </c>
@@ -1505,6 +1659,9 @@
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:5">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
       <c r="B24" s="7" t="s">
         <v>41</v>
       </c>
@@ -1517,20 +1674,24 @@
       <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:5">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
       <c r="B25" s="14" t="s">
         <v>42</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:5">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
       <c r="B26" s="14" t="s">
         <v>43</v>
       </c>
@@ -1541,6 +1702,9 @@
       <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:5">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
       <c r="B27" s="14" t="s">
         <v>45</v>
       </c>
@@ -1551,6 +1715,9 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
       <c r="B28" s="14" t="s">
         <v>46</v>
       </c>
@@ -1563,46 +1730,88 @@
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="B29" s="7"/>
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="C29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="8"/>
+      <c r="D29" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="B30" s="7"/>
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>50</v>
+      </c>
       <c r="C30" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="8"/>
+      <c r="D30" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="B31" s="7"/>
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>52</v>
+      </c>
       <c r="C31" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="7"/>
-      <c r="E31" s="8"/>
+      <c r="E31" s="15" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="B32" s="7"/>
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>55</v>
+      </c>
       <c r="C32" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="7"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="2:5">
-      <c r="B33" s="7"/>
+      <c r="E32" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="C33" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D33" s="7"/>
+      <c r="D33" s="16" t="s">
+        <v>57</v>
+      </c>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="1:5">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7" t="s">
         <v>17</v>
@@ -1610,7 +1819,10 @@
       <c r="D34" s="7"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="1:5">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7" t="s">
         <v>17</v>
@@ -1618,43 +1830,43 @@
       <c r="D35" s="7"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="1:5">
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="1:5">
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="1:5">
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="1:5">
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="1:5">
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="1:5">
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="1:5">
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="1:5">
       <c r="E43" s="2"/>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="1:5">
       <c r="E44" s="2"/>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" spans="1:5">
       <c r="E45" s="2"/>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="1:5">
       <c r="E46" s="2"/>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" spans="1:5">
       <c r="E47" s="2"/>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="1:5">
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="5:5">
@@ -1815,12 +2027,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1829,12 +2041,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1844,12 +2056,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A17" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>